<commit_message>
update requirments, rename project_info, update contract_reconciler.py
</commit_message>
<xml_diff>
--- a/master_data/contract_data.xlsx
+++ b/master_data/contract_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmuther/Dev/Learn/python/contract_reconciler_231224/master_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEDDAFE3-24DE-CD4B-AA8C-34866D3312EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9BCDB9-1180-A746-B6E0-32C75667C36E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32640" yWindow="-12920" windowWidth="26780" windowHeight="15940" xr2:uid="{2F3A525F-2EC4-5B40-A161-3DF563C03C52}"/>
+    <workbookView xWindow="14300" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{2F3A525F-2EC4-5B40-A161-3DF563C03C52}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -195,19 +195,19 @@
     <t>AAA Widgets, Inc</t>
   </si>
   <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>SEA</t>
-  </si>
-  <si>
-    <t>ESA</t>
-  </si>
-  <si>
-    <t>Co. #</t>
-  </si>
-  <si>
-    <t>Company</t>
+    <t>Co. Number</t>
+  </si>
+  <si>
+    <t>Co. Name</t>
+  </si>
+  <si>
+    <t>ESA Required</t>
+  </si>
+  <si>
+    <t>SEA Required</t>
+  </si>
+  <si>
+    <t>Contact Email</t>
   </si>
 </sst>
 </file>
@@ -573,32 +573,32 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -608,10 +608,10 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -625,10 +625,10 @@
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -642,10 +642,10 @@
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -659,10 +659,10 @@
       <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -676,10 +676,10 @@
       <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -693,10 +693,10 @@
       <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -710,10 +710,10 @@
       <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -727,10 +727,10 @@
       <c r="B9" s="2">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -744,10 +744,10 @@
       <c r="B10" s="2">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -761,10 +761,10 @@
       <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -778,10 +778,10 @@
       <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -795,10 +795,10 @@
       <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -812,10 +812,10 @@
       <c r="B14" s="2">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -829,10 +829,10 @@
       <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
@@ -844,10 +844,10 @@
       <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
@@ -859,10 +859,10 @@
       <c r="B17" s="2">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1"/>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
         <v>21</v>
       </c>
@@ -874,8 +874,8 @@
       <c r="B18" s="2">
         <v>17</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -889,8 +889,8 @@
       <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -904,8 +904,8 @@
       <c r="B20" s="2">
         <v>19</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -919,8 +919,8 @@
       <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -934,8 +934,8 @@
       <c r="B22" s="2">
         <v>21</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -949,8 +949,8 @@
       <c r="B23" s="2">
         <v>22</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -964,8 +964,8 @@
       <c r="B24" s="2">
         <v>23</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -979,8 +979,8 @@
       <c r="B25" s="2">
         <v>24</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -994,8 +994,8 @@
       <c r="B26" s="2">
         <v>25</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -1009,8 +1009,8 @@
       <c r="B27" s="2">
         <v>26</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -1019,5 +1019,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>